<commit_message>
Refreshed Raw, Doc, PDF
</commit_message>
<xml_diff>
--- a/errors.xlsx
+++ b/errors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>КПМ-0108</t>
+          <t>КПМ-0273</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,55 +460,55 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>КПМ-0244</t>
+          <t>КПМ-0283</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['Некорректный термин соответствия для результата 1']</t>
+          <t>['Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>КПМ-0245</t>
+          <t>КПМ-0285</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['Некорректный термин соответствия для результата 1']</t>
+          <t>['Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>КПМ-0246</t>
+          <t>КПМ-0286</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['Некорректный термин соответствия для результата 1']</t>
+          <t>['Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>КПМ-0258</t>
+          <t>КПМ-0287</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['Некорректный термин соответствия для результата 1']</t>
+          <t>['Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>КПМ-0262</t>
+          <t>КПМ-0289</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,19 +520,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>КПМ-0268</t>
+          <t>КПМ-0291</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['Некорректный термин соответствия для результата 1']</t>
+          <t>['Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>КПМ-0273</t>
+          <t>КПМ-0292</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>КПМ-0283</t>
+          <t>КПМ-0293</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>КПМ-0285</t>
+          <t>КПМ-0294</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>КПМ-0286</t>
+          <t>КПМ-0295</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,19 +580,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>КПМ-0287</t>
+          <t>КПМ-0296</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['Некорректный термин соответствия для результата 1', 'Не выбрано ни одной проблемы']</t>
+          <t>['Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>КПМ-0289</t>
+          <t>КПМ-0341</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>КПМ-0291</t>
+          <t>КПМ-0363</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,19 +616,19 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>КПМ-0292</t>
+          <t>Лаб-2022-10</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['Не выбрано ни одной проблемы']</t>
+          <t>['Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>КПМ-0293</t>
+          <t>Лаб-2022-12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,19 +640,19 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>КПМ-0294</t>
+          <t>Лаб-2022-14</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['Не выбрано ни одной проблемы']</t>
+          <t>['Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>КПМ-0295</t>
+          <t>Лаб-2022-17</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>КПМ-0296</t>
+          <t>Лаб-2022-18</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,19 +676,19 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>КПМ-0297</t>
+          <t>Лаб-2022-2</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['Некорректный термин соответствия для результата 1', 'Некорректный термин соответствия для результата 2', 'Не выбрано ни одной проблемы']</t>
+          <t>['Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>КПМ-0341</t>
+          <t>Лаб-2022-21</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -700,132 +700,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>КПМ-0346</t>
+          <t>Лаб-2022-34</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>КПМ-0363</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Лаб-2022-10</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Лаб-2022-12</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Лаб-2022-14</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Лаб-2022-17</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Лаб-2022-18</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Лаб-2022-2</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы', 'Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Лаб-2022-21</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Лаб-2022-34</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>['Не выбрано ни одной проблемы']</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Лаб-2022-41</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>['Ошибка в ДОК для результата 1']</t>
+          <t>['Не выбрано ни одной проблемы']</t>
         </is>
       </c>
     </row>

</xml_diff>